<commit_message>
Additional test cases and test template
</commit_message>
<xml_diff>
--- a/src/main/java/resources/credentials.xlsx
+++ b/src/main/java/resources/credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnowaczyk2\Desktop\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnowaczyk2\Desktop\Resources\workspace\SeleniumTestProject1\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8070990B-F8B7-425D-AEA1-078355D59992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AC8C8A-F353-4A70-A85D-945C092B2225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,16 +73,16 @@
     <t>bogdan.romanski@test.com</t>
   </si>
   <si>
-    <t>wojciech.giernacki@test.com</t>
-  </si>
-  <si>
     <t>letmein123</t>
   </si>
   <si>
     <t>counttothree123</t>
   </si>
   <si>
-    <t>technicalguy1</t>
+    <t>marin.kozieradka@test.com</t>
+  </si>
+  <si>
+    <t>koziol333</t>
   </si>
 </sst>
 </file>
@@ -412,17 +412,17 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -447,7 +447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -458,7 +458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -469,7 +469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -480,40 +480,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>12</v>
       </c>
@@ -522,7 +522,7 @@
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{45BE9DC0-B994-47B1-BB67-7EDEF43B16FE}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{F7B308AC-5B01-4142-BC62-65909799D384}"/>
-    <hyperlink ref="A8" r:id="rId3" xr:uid="{D66929FE-E2FB-4F90-8ABD-6B98380AE88C}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{4246D450-D947-4449-B0D1-88FB54FFB133}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
@@ -535,7 +535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>